<commit_message>
added code to remove empty datasets from mnova json so that data is not overwritten
</commit_message>
<xml_diff>
--- a/exampleProblems/2-ethyl-1-indanone/2-ethyl-1-indanone.xlsx
+++ b/exampleProblems/2-ethyl-1-indanone/2-ethyl-1-indanone.xlsx
@@ -8,20 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="1" r:id="rId1"/>
-    <sheet name="H1_1D" sheetId="2" r:id="rId2"/>
-    <sheet name="H1_pureshift" sheetId="3" r:id="rId3"/>
-    <sheet name="C13_1D" sheetId="4" r:id="rId4"/>
-    <sheet name="COSY" sheetId="5" r:id="rId5"/>
-    <sheet name="HMBC" sheetId="6" r:id="rId6"/>
-    <sheet name="HSQC" sheetId="7" r:id="rId7"/>
-    <sheet name="NOESY" sheetId="8" r:id="rId8"/>
+    <sheet name="C13_1D" sheetId="2" r:id="rId2"/>
+    <sheet name="COSY" sheetId="3" r:id="rId3"/>
+    <sheet name="HMBC" sheetId="4" r:id="rId4"/>
+    <sheet name="HSQC" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>smiles</t>
   </si>
@@ -425,54 +422,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:4">
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:4">
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -649,9 +598,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -676,13 +625,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.738430033265081</v>
+        <v>7.566996222976494</v>
       </c>
       <c r="C2">
-        <v>7.348358839227305</v>
+        <v>7.447310850078518</v>
       </c>
       <c r="D2">
-        <v>0.8134750127792358</v>
+        <v>1.574164390563965</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -696,10 +645,10 @@
         <v>7.566996222976494</v>
       </c>
       <c r="C3">
-        <v>7.447310850078518</v>
+        <v>7.350210639609407</v>
       </c>
       <c r="D3">
-        <v>1.574164390563965</v>
+        <v>0.2207812666893005</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -710,13 +659,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.566996222976494</v>
+        <v>3.310011683794853</v>
       </c>
       <c r="C4">
-        <v>7.350210639609407</v>
+        <v>2.606743400116869</v>
       </c>
       <c r="D4">
-        <v>0.2207812666893005</v>
+        <v>0.05913177505135536</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -727,13 +676,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3.30728647990954</v>
+        <v>1.965567855644642</v>
       </c>
       <c r="C5">
-        <v>2.812258357628771</v>
+        <v>2.605891541783929</v>
       </c>
       <c r="D5">
-        <v>0.3013738095760345</v>
+        <v>0.3139396905899048</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -744,13 +693,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.307057782702674</v>
+        <v>1.965477164626156</v>
       </c>
       <c r="C6">
-        <v>2.607530136577619</v>
+        <v>1.001326068172147</v>
       </c>
       <c r="D6">
-        <v>0.09333708882331848</v>
+        <v>0.8830317854881287</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -761,49 +710,15 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.965567855644642</v>
+        <v>1.965097083513452</v>
       </c>
       <c r="C7">
-        <v>2.605891541783929</v>
+        <v>1.964488317301542</v>
       </c>
       <c r="D7">
-        <v>0.3139396905899048</v>
+        <v>0.1004290208220482</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1.965477164626156</v>
-      </c>
-      <c r="C8">
-        <v>1.001326068172147</v>
-      </c>
-      <c r="D8">
-        <v>0.8830317854881287</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1.965097083513452</v>
-      </c>
-      <c r="C9">
-        <v>1.964488317301542</v>
-      </c>
-      <c r="D9">
-        <v>0.1004290208220482</v>
-      </c>
-      <c r="E9">
         <v>0</v>
       </c>
     </row>
@@ -812,7 +727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
@@ -1434,7 +1349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1629,31 +1544,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed colour scheme for colour blind people
</commit_message>
<xml_diff>
--- a/exampleProblems/2-ethyl-1-indanone/2-ethyl-1-indanone.xlsx
+++ b/exampleProblems/2-ethyl-1-indanone/2-ethyl-1-indanone.xlsx
@@ -507,22 +507,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7.737906072649333</v>
+        <v>7.737272812743949</v>
       </c>
       <c r="C2" t="n">
-        <v>1.000033224208112</v>
+        <v>0.9831644498137422</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ddq</t>
+          <t>ddt</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.574, 1.25, 7.69</t>
+          <t>0.648, 1.29, 7.67</t>
         </is>
       </c>
     </row>
@@ -531,22 +531,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7.567027089863733</v>
+        <v>7.566881170536674</v>
       </c>
       <c r="C3" t="n">
-        <v>1.044540291933063</v>
+        <v>1.032298456963578</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>td</t>
+          <t>ddd</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.24, 7.42</t>
+          <t>1.27, 7.23, 7.62</t>
         </is>
       </c>
     </row>
@@ -555,10 +555,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7.449204824899009</v>
+        <v>7.449063184395219</v>
       </c>
       <c r="C4" t="n">
-        <v>1.030337786233437</v>
+        <v>1.02813288006641</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -570,7 +570,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.953, 7.68</t>
+          <t>0.958, 7.68</t>
         </is>
       </c>
     </row>
@@ -579,22 +579,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>7.349303067688013</v>
+        <v>7.348598146833025</v>
       </c>
       <c r="C5" t="n">
-        <v>1.048615790009063</v>
+        <v>0.9976276316100109</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ddt</t>
+          <t>ddq</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.855, 7.22, 8.52</t>
+          <t>0.853, 7.18, 7.6</t>
         </is>
       </c>
     </row>
@@ -603,10 +603,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.308352426774753</v>
+        <v>3.308244907884105</v>
       </c>
       <c r="C6" t="n">
-        <v>1.051625801961403</v>
+        <v>1.018912934186621</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -618,7 +618,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.777, 7.89, 17.1</t>
+          <t>0.793, 7.87, 17.1</t>
         </is>
       </c>
     </row>
@@ -627,58 +627,50 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.812059483796793</v>
+        <v>2.815544050454685</v>
       </c>
       <c r="C7" t="n">
-        <v>1.049047504685912</v>
+        <v>0.9721759318922879</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>dd</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3.92, 17.1</t>
-        </is>
-      </c>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2.606421855689738</v>
+        <v>2.607303542092875</v>
       </c>
       <c r="C8" t="n">
-        <v>1.047623487581841</v>
+        <v>1.063308934024798</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dddd</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>3.92, 4.59, 7.86, 9.14</t>
-        </is>
-      </c>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1.965223914004773</v>
+        <v>1.965073516532478</v>
       </c>
       <c r="C9" t="n">
-        <v>1.058717568990737</v>
+        <v>1.092167043574244</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -690,7 +682,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4.56, 7.5, 13.7</t>
+          <t>4.58, 7.51, 13.7</t>
         </is>
       </c>
     </row>
@@ -699,30 +691,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1.533649712037166</v>
+        <v>1.531828172669145</v>
       </c>
       <c r="C10" t="n">
-        <v>1.082174127577414</v>
+        <v>0.9708400807358168</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>ddq</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>7.33, 9.11, 13.7</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1.001752588817867</v>
+        <v>1.001636089631483</v>
       </c>
       <c r="C11" t="n">
-        <v>3.160296209296122</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
@@ -734,7 +730,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>7.42</t>
+          <t>7.41</t>
         </is>
       </c>
     </row>
@@ -1201,13 +1197,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.311021822079599</v>
+        <v>3.308415120635955</v>
       </c>
       <c r="C5" t="n">
-        <v>2.608015572186058</v>
+        <v>2.605142644437138</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05912093073129654</v>
+        <v>0.0933314710855484</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1928,7 +1924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1963,13 +1959,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7.737564351158939</v>
+        <v>3.309042826572111</v>
       </c>
       <c r="C2" t="n">
-        <v>123.8337323956202</v>
+        <v>32.31545964835274</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4917645454406738</v>
+        <v>-0.2761878371238708</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1980,13 +1976,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7.567158389420261</v>
+        <v>2.809725261777252</v>
       </c>
       <c r="C3" t="n">
-        <v>134.5965624357195</v>
+        <v>32.3204001435485</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4680789709091187</v>
+        <v>-0.005617320537567139</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1997,134 +1993,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7.448374359487117</v>
+        <v>1.001847641444521</v>
       </c>
       <c r="C4" t="n">
-        <v>126.5161608056142</v>
+        <v>11.58371917677896</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5304826498031616</v>
+        <v>1.686318397521973</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>7.352275399932183</v>
-      </c>
-      <c r="C5" t="n">
-        <v>127.2695589084211</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.7418267726898193</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>3.30748707389514</v>
-      </c>
-      <c r="C6" t="n">
-        <v>32.32275480793425</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.2879419922828674</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2.812951456977248</v>
-      </c>
-      <c r="C7" t="n">
-        <v>32.32275480793425</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.005584955215454102</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2.606848512273122</v>
-      </c>
-      <c r="C8" t="n">
-        <v>48.75260384447412</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.5183935165405273</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1.964517682293971</v>
-      </c>
-      <c r="C9" t="n">
-        <v>24.42621553029936</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.4160599112510681</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.532973524629702</v>
-      </c>
-      <c r="C10" t="n">
-        <v>24.46333319880646</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.2256830930709839</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1.001844729650673</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11.59013571628115</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.684660077095032</v>
-      </c>
-      <c r="E11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>